<commit_message>
fixing the ordering for the pilot
</commit_message>
<xml_diff>
--- a/scripts/RadLab - All Experiments.xlsx
+++ b/scripts/RadLab - All Experiments.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arda/Obsidian/Research/RadLab/Meta-analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arda/GitHub/RadLab/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A18FB8-FC9E-814F-92DE-E8C470238B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C05654-C588-104D-8B22-3E26C7A01EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -564,7 +564,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>